<commit_message>
Commit 190312  Update attendance_management.ejs attendance_management.js  Update collection_attendances_migration.xlsx
</commit_message>
<xml_diff>
--- a/collection_attendances_migration.xlsx
+++ b/collection_attendances_migration.xlsx
@@ -16,34 +16,35 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-01"), start_time:new Date("2019-02-01T09:00:00Z"), end_time:new Date("2019-02-01T17:45:00Z"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-02"), start_time:new Date("2019-02-02T09:00:00Z"), end_time:new Date("2019-02-02T17:45:00Z"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-03"), start_time:new Date("2019-02-03T09:00:00Z"), end_time:new Date("2019-02-03T17:45:00Z"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-04"), start_time:new Date("2019-02-04T09:00:00Z"), end_time:new Date("2019-02-04T17:45:00Z"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-05"), start_time:new Date("2019-02-05T09:00:00Z"), end_time:new Date("2019-02-05T17:45:00Z"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-06"), start_time:new Date("2019-02-06T09:00:00Z"), end_time:new Date("2019-02-06T17:45:00Z"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-07"), start_time:new Date("2019-02-07T09:00:00Z"), end_time:new Date("2019-02-07T17:45:00Z"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-08"), start_time:new Date("2019-02-08T09:00:00Z"), end_time:new Date("2019-02-08T17:45:00Z"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-09"), start_time:new Date("2019-02-09T09:00:00Z"), end_time:new Date("2019-02-09T17:45:00Z"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-10"), start_time:new Date("2019-02-10T09:00:00Z"), end_time:new Date("2019-02-10T17:45:00Z"), message:"" }, {unique:true})</t>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-01"), start_time:new Date("2019-02-01 09:00:00"), end_time:new Date("2019-02-01 17:45:00"), message:"" }, {unique:true})</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-02"), start_time:new Date("2019-02-02 09:00:00"), end_time:new Date("2019-02-02 17:45:00"), message:"" }, {unique:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-03"), start_time:new Date("2019-02-03 09:00:00"), end_time:new Date("2019-02-03 17:45:00"), message:"" }, {unique:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-04"), start_time:new Date("2019-02-04 09:00:00"), end_time:new Date("2019-02-04 17:45:00"), message:"" }, {unique:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-05"), start_time:new Date("2019-02-05 09:00:00"), end_time:new Date("2019-02-05 17:45:00"), message:"" }, {unique:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-06"), start_time:new Date("2019-02-06 09:00:00"), end_time:new Date("2019-02-06 17:45:00"), message:"" }, {unique:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-07"), start_time:new Date("2019-02-07 09:00:00"), end_time:new Date("2019-02-07 17:45:00"), message:"" }, {unique:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-08"), start_time:new Date("2019-02-08 09:00:00"), end_time:new Date("2019-02-08 17:45:00"), message:"" }, {unique:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-09"), start_time:new Date("2019-02-09 09:00:00"), end_time:new Date("2019-02-09 17:45:00"), message:"" }, {unique:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-10"), start_time:new Date("2019-02-10 09:00:00"), end_time:new Date("2019-02-10 17:45:00"), message:"" }, {unique:true})</t>
   </si>
 </sst>
 </file>
@@ -397,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Commit 190402  -Update DB Migration
</commit_message>
<xml_diff>
--- a/collection_attendances_migration.xlsx
+++ b/collection_attendances_migration.xlsx
@@ -14,37 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-01"), start_time:new Date("2019-02-01 09:00:00"), end_time:new Date("2019-02-01 17:45:00"), message:"" }, {unique:true})</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-02"), start_time:new Date("2019-02-02 09:00:00"), end_time:new Date("2019-02-02 17:45:00"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-03"), start_time:new Date("2019-02-03 09:00:00"), end_time:new Date("2019-02-03 17:45:00"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-04"), start_time:new Date("2019-02-04 09:00:00"), end_time:new Date("2019-02-04 17:45:00"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-05"), start_time:new Date("2019-02-05 09:00:00"), end_time:new Date("2019-02-05 17:45:00"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-06"), start_time:new Date("2019-02-06 09:00:00"), end_time:new Date("2019-02-06 17:45:00"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-07"), start_time:new Date("2019-02-07 09:00:00"), end_time:new Date("2019-02-07 17:45:00"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-08"), start_time:new Date("2019-02-08 09:00:00"), end_time:new Date("2019-02-08 17:45:00"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-09"), start_time:new Date("2019-02-09 09:00:00"), end_time:new Date("2019-02-09 17:45:00"), message:"" }, {unique:true})</t>
-  </si>
-  <si>
-    <t>db.attendances_201902.insert({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-10"), start_time:new Date("2019-02-10 09:00:00"), end_time:new Date("2019-02-10 17:45:00"), message:"" }, {unique:true})</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>db.attendances_201902.update({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-02")}, {mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-02"), start_time:new Date("2019-02-02 09:00:00"), end_time:new Date("2019-02-02 17:45:00"), message:"" }, {upsert:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.update({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-03")}, {mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-03"), start_time:new Date("2019-02-03 09:00:00"), end_time:new Date("2019-02-03 17:45:00"), message:"" }, {upsert:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.update({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-04")}, {mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-04"), start_time:new Date("2019-02-04 09:00:00"), end_time:new Date("2019-02-04 17:45:00"), message:"" }, {upsert:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.update({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-05")}, {mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-05"), start_time:new Date("2019-02-05 09:00:00"), end_time:new Date("2019-02-05 17:45:00"), message:"" }, {upsert:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.update({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-06")}, {mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-06"), start_time:new Date("2019-02-06 09:00:00"), end_time:new Date("2019-02-06 17:45:00"), message:"" }, {upsert:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.update({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-07")}, {mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-07"), start_time:new Date("2019-02-07 09:00:00"), end_time:new Date("2019-02-07 17:45:00"), message:"" }, {upsert:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.update({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-08")}, {mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-08"), start_time:new Date("2019-02-08 09:00:00"), end_time:new Date("2019-02-08 17:45:00"), message:"" }, {upsert:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.update({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-09")}, {mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-09"), start_time:new Date("2019-02-09 09:00:00"), end_time:new Date("2019-02-09 17:45:00"), message:"" }, {upsert:true})</t>
+  </si>
+  <si>
+    <t>db.attendances_201902.update({mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-10")}, {mail:'ys-yoo@softwiz.jp', date:new Date("2019-02-10"), start_time:new Date("2019-02-10 09:00:00"), end_time:new Date("2019-02-10 17:45:00"), message:"" }, {upsert:true})</t>
   </si>
 </sst>
 </file>
@@ -398,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -453,9 +449,7 @@
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
Commit 190404  -Update attendance_management.ejs and attendance_management.js
</commit_message>
<xml_diff>
--- a/collection_attendances_migration.xlsx
+++ b/collection_attendances_migration.xlsx
@@ -404,8 +404,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>